<commit_message>
Update document and data set
</commit_message>
<xml_diff>
--- a/MiningTopKCoOccurrenceItemsConsole/testResults/PreprocessingMemUsage.xlsx
+++ b/MiningTopKCoOccurrenceItemsConsole/testResults/PreprocessingMemUsage.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="connect" sheetId="1" r:id="rId1"/>
     <sheet name="syn_data1" sheetId="3" r:id="rId2"/>
     <sheet name="syn_data2" sheetId="4" r:id="rId3"/>
-    <sheet name="accidents" sheetId="2" r:id="rId4"/>
+    <sheet name="T10I4D100K" sheetId="5" r:id="rId4"/>
+    <sheet name="kosarak" sheetId="6" r:id="rId5"/>
+    <sheet name="accidents" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="14">
   <si>
     <t>K=1</t>
   </si>
@@ -1557,7 +1559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AQ7"/>
     </sheetView>
   </sheetViews>
@@ -1947,6 +1949,792 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AQ7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AQ7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="L3" s="1">
+        <v>3</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="W3" s="1">
+        <v>3</v>
+      </c>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AH3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="L4" s="1">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="W4" s="1">
+        <v>4</v>
+      </c>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AH4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="L5" s="1">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="W5" s="1">
+        <v>5</v>
+      </c>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AH5" s="1">
+        <v>5</v>
+      </c>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="L6" s="1">
+        <v>6</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="W6" s="1">
+        <v>6</v>
+      </c>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AH6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="L7" s="1">
+        <v>7</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="W7" s="1">
+        <v>7</v>
+      </c>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AH7" s="1">
+        <v>7</v>
+      </c>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AQ7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AQ7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="L3" s="1">
+        <v>3</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="W3" s="1">
+        <v>3</v>
+      </c>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AH3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="1"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="L4" s="1">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="W4" s="1">
+        <v>4</v>
+      </c>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AH4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="1"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="L5" s="1">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="W5" s="1">
+        <v>5</v>
+      </c>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AH5" s="1">
+        <v>5</v>
+      </c>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="L6" s="1">
+        <v>6</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="W6" s="1">
+        <v>6</v>
+      </c>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AH6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="1"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
+    </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="L7" s="1">
+        <v>7</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="W7" s="1">
+        <v>7</v>
+      </c>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AH7" s="1">
+        <v>7</v>
+      </c>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="1"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update all chart result
</commit_message>
<xml_diff>
--- a/MiningTopKCoOccurrenceItemsConsole/testResults/PreprocessingMemUsage.xlsx
+++ b/MiningTopKCoOccurrenceItemsConsole/testResults/PreprocessingMemUsage.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cao hoc\Codes\Mining-Top-K-Co-Occurrence-Items\MiningTopKCoOccurrenceItemsConsole\testResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ay\Documents\GitHub\Mining-Top-K-Co-Occurrence-Items\MiningTopKCoOccurrenceItemsConsole\testResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="connect" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="14">
   <si>
     <t>K=1</t>
   </si>
@@ -121,10 +121,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,6 +141,3580 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>connect!$A$11:$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>NT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NTI</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BT</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BTI</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BTIV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>connect!$A$12:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>442</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>380</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="7762872"/>
+        <c:axId val="7765224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="7762872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7765224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="7765224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="7762872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>syn_data1!$A$11:$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>NT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NTI</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BT</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BTI</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BTIV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>syn_data1!$A$12:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1433.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2150.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3686.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1740.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2150.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2150.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="359039816"/>
+        <c:axId val="359038640"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="359039816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359038640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="359038640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359039816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>syn_data2!$A$11:$F$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>NT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NTI</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BT</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BTI</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BTIV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>syn_data2!$A$12:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1331.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3788.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1638.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2048</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="359037464"/>
+        <c:axId val="359047264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="359037464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359047264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="359047264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="359037464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>accidents!$A$12:$F$12</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>NT</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NTI</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>PT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>BT</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BTI</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>BTIV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>accidents!$A$13:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>799</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1126.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>1228.8</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>1126.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>1166.0999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="265025392"/>
+        <c:axId val="265021080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="265025392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="265021080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="265021080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Memory</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (MB)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="265025392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>41275</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>225425</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,53 +3980,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ7"/>
+  <dimension ref="A1:AQ12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.453125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.453125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.7265625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3.453125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.453125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.7265625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.453125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.453125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="7" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="3.7265625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +4040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -587,7 +4162,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -701,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -815,7 +4390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -929,7 +4504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1043,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1155,24 +4730,65 @@
       </c>
       <c r="AQ7" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>212</v>
+      </c>
+      <c r="B12">
+        <v>386</v>
+      </c>
+      <c r="C12">
+        <v>240</v>
+      </c>
+      <c r="D12">
+        <v>365</v>
+      </c>
+      <c r="E12">
+        <v>442</v>
+      </c>
+      <c r="F12">
+        <v>380</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ7"/>
+  <dimension ref="A1:AQ12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AQ7"/>
+      <selection activeCell="A11" sqref="A11:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1186,7 +4802,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1300,7 +4916,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -1350,7 +4966,7 @@
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -1400,7 +5016,7 @@
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -1450,7 +5066,7 @@
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1500,7 +5116,7 @@
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1550,22 +5166,69 @@
       <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
     </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <f>1.4*1024</f>
+        <v>1433.6</v>
+      </c>
+      <c r="B12" s="3">
+        <f>2.1*1024</f>
+        <v>2150.4</v>
+      </c>
+      <c r="C12" s="3">
+        <f>3.6*1024</f>
+        <v>3686.4</v>
+      </c>
+      <c r="D12" s="3">
+        <f>1.7*1024</f>
+        <v>1740.8</v>
+      </c>
+      <c r="E12" s="3">
+        <f>2.1*1024</f>
+        <v>2150.4</v>
+      </c>
+      <c r="F12" s="3">
+        <f>2.1*1024</f>
+        <v>2150.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ7"/>
+  <dimension ref="A1:AQ12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AQ7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1579,7 +5242,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1693,7 +5356,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -1743,7 +5406,7 @@
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -1793,7 +5456,7 @@
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -1843,7 +5506,7 @@
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -1893,7 +5556,7 @@
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -1943,8 +5606,55 @@
       <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
     </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <f>1.3*1024</f>
+        <v>1331.2</v>
+      </c>
+      <c r="B12" s="3">
+        <f>2*1024</f>
+        <v>2048</v>
+      </c>
+      <c r="C12" s="3">
+        <f>3.7*1024</f>
+        <v>3788.8</v>
+      </c>
+      <c r="D12" s="3">
+        <f>1024*1.6</f>
+        <v>1638.4</v>
+      </c>
+      <c r="E12" s="3">
+        <f>1024*2</f>
+        <v>2048</v>
+      </c>
+      <c r="F12" s="3">
+        <f>1024*2</f>
+        <v>2048</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1956,9 +5666,9 @@
       <selection sqref="A1:AQ7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +5682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -2086,7 +5796,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -2136,7 +5846,7 @@
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -2186,7 +5896,7 @@
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -2236,7 +5946,7 @@
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -2286,7 +5996,7 @@
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -2345,13 +6055,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AQ7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2365,7 +6075,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -2479,7 +6189,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -2529,7 +6239,7 @@
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -2579,7 +6289,7 @@
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -2629,7 +6339,7 @@
       <c r="AP5" s="1"/>
       <c r="AQ5" s="1"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -2679,7 +6389,7 @@
       <c r="AP6" s="1"/>
       <c r="AQ6" s="1"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -2736,25 +6446,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ7"/>
+  <dimension ref="A1:AQ13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" customWidth="1"/>
+    <col min="3" max="3" width="5.54296875" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2768,7 +6478,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2890,7 +6600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -3004,7 +6714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -3118,7 +6828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -3232,7 +6942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -3346,7 +7056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -3458,9 +7168,55 @@
       </c>
       <c r="AQ7" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>799</v>
+      </c>
+      <c r="B13" s="3">
+        <f>1.1*1024</f>
+        <v>1126.4000000000001</v>
+      </c>
+      <c r="C13">
+        <f>1.2*1024</f>
+        <v>1228.8</v>
+      </c>
+      <c r="D13">
+        <f>1.1*1024</f>
+        <v>1126.4000000000001</v>
+      </c>
+      <c r="E13">
+        <f>1.25*1024</f>
+        <v>1280</v>
+      </c>
+      <c r="F13">
+        <f>1.15*1014</f>
+        <v>1166.0999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>